<commit_message>
#37962 コンボと、判定表示のON/OFF機能を追加。CONFIGURATION / Drums (やGuitar, Bass) / Display Options / DisplayComboやDisplayJudgeで設定する。
</commit_message>
<xml_diff>
--- a/RuntimeResources/System/resources.xlsx
+++ b/RuntimeResources/System/resources.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="971">
   <si>
     <t xml:space="preserve">stringName</t>
   </si>
@@ -830,6 +830,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DTXMania</t>
     </r>
@@ -838,6 +839,7 @@
         <sz val="10"/>
         <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">起動時に、強制的に電源プランを「高パフォーマンス」にします。</t>
     </r>
@@ -846,6 +848,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">\n
 (DTXMania</t>
@@ -855,6 +858,7 @@
         <sz val="10"/>
         <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">終了時、電源プランは元に戻ります</t>
     </r>
@@ -863,6 +867,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)\n
 \n
@@ -873,6 +878,7 @@
         <sz val="10"/>
         <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">機能を搭載する</t>
     </r>
@@ -881,6 +887,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">PC</t>
     </r>
@@ -889,6 +896,7 @@
         <sz val="10"/>
         <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">や、</t>
     </r>
@@ -897,6 +905,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Windows10(1709)</t>
     </r>
@@ -905,6 +914,7 @@
         <sz val="10"/>
         <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">以降の環境では、この設定は無視されます。</t>
     </r>
@@ -2912,6 +2922,21 @@
     <t xml:space="preserve">DisplayCombo</t>
   </si>
   <si>
+    <t xml:space="preserve">To show, or NOT to show, the Combo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">演奏時のコンボ文字列の表示有無を指定します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">左,中心,右,关</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//strCfgDrComboPosition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ComboPosition</t>
+  </si>
+  <si>
     <t xml:space="preserve">The display position for Drums Combo.</t>
   </si>
   <si>
@@ -2990,13 +3015,40 @@
     <t xml:space="preserve">演奏時のドラムコンボ文字列の位置を指定します。</t>
   </si>
   <si>
-    <t xml:space="preserve">左,中心,右,关</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//strCfgDrComboPosition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ComboPosition</t>
+    <t xml:space="preserve">strCfgDrCombo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrumsCombo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To show, or NOT to show, the Drums Combo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFF,ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">演奏時のドラムコンボ文字列を表示するかどうかを指定します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GuitarCombo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To show, or NOT to show, the Guitar Combo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">演奏時のギターコンボ文字列を表示するかどうかを指定します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strCfgBsCombo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BassCombo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To show, or NOT to show, the Bass Combo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">演奏時のベースコンボ文字列を表示するかどうかを指定します。</t>
   </si>
   <si>
     <t xml:space="preserve">strCfgDgbDisplayJudge</t>
@@ -3014,7 +3066,7 @@
     <t xml:space="preserve">//strCfgDrJudgePosition</t>
   </si>
   <si>
-    <t xml:space="preserve">JudgePosition</t>
+    <t xml:space="preserve">DrumsJudgePosition</t>
   </si>
   <si>
     <t xml:space="preserve">The position to show judgement mark.\n
@@ -3084,6 +3136,9 @@
   </si>
   <si>
     <t xml:space="preserve">//strCfgGtJudgePosition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GuitarJudgePosition</t>
   </si>
   <si>
     <t xml:space="preserve">The position to show judgement mark.\n
@@ -3155,6 +3210,9 @@
   </si>
   <si>
     <t xml:space="preserve">//strCfgBsJudgePosition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BassJudgePosition</t>
   </si>
   <si>
     <t xml:space="preserve">ベースの判定文字の表示位置を指定します。\n
@@ -4800,7 +4858,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -4858,16 +4916,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
@@ -4923,7 +4971,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4960,15 +5008,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5053,10 +5097,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J304"/>
+  <dimension ref="A1:J307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D160" activeCellId="0" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5749,10 +5793,10 @@
       <c r="B56" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F56" s="5" t="s">
         <v>153</v>
       </c>
     </row>
@@ -6307,7 +6351,7 @@
       <c r="F95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="9" t="s">
         <v>309</v>
       </c>
       <c r="B96" s="6" t="s">
@@ -6321,7 +6365,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="10"/>
+      <c r="A97" s="9"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="F97" s="6"/>
@@ -6562,7 +6606,7 @@
       <c r="B116" s="6"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="10" t="s">
+      <c r="A118" s="9" t="s">
         <v>373</v>
       </c>
       <c r="B118" s="6" t="s">
@@ -7050,1740 +7094,1792 @@
       <c r="C160" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="D160" s="6" t="s">
+      <c r="D160" s="6"/>
+      <c r="F160" s="0" t="s">
         <v>494</v>
       </c>
-      <c r="F160" s="0" t="s">
+      <c r="J160" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="J160" s="4" t="s">
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="9" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="10" t="s">
+      <c r="B161" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="B161" s="10" t="s">
+      <c r="C161" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="C161" s="6" t="s">
-        <v>493</v>
-      </c>
       <c r="D161" s="6" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="F161" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="J161" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="J161" s="4" t="s">
-        <v>496</v>
-      </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="B162" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="C162" s="0" t="s">
+      <c r="A162" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="F162" s="0" t="s">
+      <c r="B162" s="9" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="163" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
+      <c r="C162" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="B163" s="0" t="s">
+      <c r="D162" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="C163" s="8" t="s">
+      <c r="F162" s="6" t="s">
         <v>505</v>
       </c>
+      <c r="J162" s="4"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>507</v>
+      </c>
       <c r="D163" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="F163" s="8" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="F163" s="6" t="s">
         <v>508</v>
       </c>
-      <c r="B164" s="0" t="s">
+      <c r="J163" s="4"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="D164" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="C164" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="D164" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="F164" s="8" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F164" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="J164" s="4"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>504</v>
-      </c>
-      <c r="C165" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="D165" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="F165" s="8" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>514</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="F165" s="0" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="D166" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="F166" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="F167" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>524</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="F167" s="8" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>520</v>
-      </c>
-      <c r="F168" s="3" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>524</v>
+      </c>
+      <c r="D168" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="F168" s="8" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>525</v>
+        <v>531</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>532</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>535</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="F173" s="8" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="B178" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>534</v>
-      </c>
-      <c r="F178" s="6" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="B179" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="C179" s="6" t="s">
-        <v>538</v>
-      </c>
-      <c r="F179" s="6" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="4" t="s">
+      <c r="B173" s="0" t="s">
         <v>540</v>
       </c>
-      <c r="B180" s="11" t="s">
+      <c r="C173" s="3" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="181" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
+      <c r="F173" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="B181" s="0" t="s">
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="C181" s="3" t="s">
+      <c r="B174" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="F181" s="3" t="s">
+    </row>
+    <row r="176" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="182" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
+      <c r="C176" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="B182" s="0" t="s">
+      <c r="F176" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="C182" s="3" t="s">
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="F182" s="3" t="s">
+      <c r="B181" s="10" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="183" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
+      <c r="C181" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="B183" s="0" t="s">
+      <c r="F181" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="C183" s="3" t="s">
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="F183" s="3" t="s">
+      <c r="B182" s="10" t="s">
         <v>553</v>
+      </c>
+      <c r="C182" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="F182" s="6" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B183" s="10" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="F195" s="3" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>587</v>
+        <v>619</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="F199" s="3" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>591</v>
+        <v>623</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="F200" s="3" t="s">
-        <v>619</v>
+        <v>625</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>620</v>
+        <v>626</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>595</v>
+        <v>627</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>621</v>
+        <v>628</v>
       </c>
       <c r="F201" s="3" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>623</v>
+        <v>630</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>624</v>
+        <v>631</v>
       </c>
       <c r="F202" s="3" t="s">
-        <v>625</v>
+        <v>632</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>626</v>
+        <v>633</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>627</v>
+        <v>634</v>
       </c>
       <c r="F203" s="3" t="s">
-        <v>628</v>
+        <v>635</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>630</v>
+        <v>637</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>632</v>
+        <v>639</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>633</v>
+        <v>640</v>
       </c>
       <c r="F205" s="3" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>635</v>
-      </c>
-      <c r="B206" s="6" t="s">
-        <v>636</v>
+        <v>642</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>619</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="F206" s="3" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>645</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>639</v>
-      </c>
-      <c r="B209" s="0" t="s">
-        <v>640</v>
-      </c>
-      <c r="C209" s="6" t="s">
-        <v>641</v>
-      </c>
-      <c r="F209" s="6" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
-        <v>643</v>
-      </c>
-      <c r="B210" s="0" t="s">
-        <v>644</v>
-      </c>
-      <c r="C210" s="6" t="s">
-        <v>645</v>
-      </c>
-      <c r="F210" s="6" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
-        <v>647</v>
-      </c>
-      <c r="B211" s="0" t="s">
-        <v>648</v>
-      </c>
-      <c r="C211" s="6" t="s">
-        <v>649</v>
-      </c>
-      <c r="F211" s="6" t="s">
-        <v>650</v>
+        <v>651</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="F209" s="3" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="C212" s="6" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="F212" s="6" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>656</v>
-      </c>
-      <c r="C213" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
+      </c>
+      <c r="C213" s="6" t="s">
+        <v>661</v>
       </c>
       <c r="F213" s="6" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="0" t="s">
-        <v>659</v>
-      </c>
-      <c r="C218" s="0" t="s">
-        <v>660</v>
-      </c>
-      <c r="F218" s="0" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
         <v>662</v>
       </c>
-      <c r="C219" s="0" t="s">
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
         <v>663</v>
       </c>
-      <c r="F219" s="0" t="s">
+      <c r="B214" s="0" t="s">
         <v>664</v>
       </c>
+      <c r="C214" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="F214" s="6" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="C215" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="F215" s="6" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="C216" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="F216" s="6" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="C221" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="F221" s="0" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="12"/>
-    </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="0" t="s">
-        <v>665</v>
-      </c>
-      <c r="B223" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="C223" s="0" t="s">
-        <v>667</v>
-      </c>
-      <c r="F223" s="0" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
-        <v>669</v>
-      </c>
-      <c r="B224" s="0" t="s">
-        <v>670</v>
-      </c>
-      <c r="C224" s="0" t="s">
-        <v>671</v>
-      </c>
-      <c r="F224" s="0" t="s">
-        <v>672</v>
+      <c r="A222" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="C222" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="F222" s="0" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="0" t="s">
-        <v>673</v>
-      </c>
-      <c r="B225" s="0" t="s">
-        <v>674</v>
-      </c>
-      <c r="C225" s="0" t="s">
-        <v>675</v>
-      </c>
-      <c r="F225" s="0" t="s">
-        <v>676</v>
-      </c>
+      <c r="C225" s="11"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="F226" s="0" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="F227" s="0" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="F228" s="0" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="F229" s="0" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="F230" s="0" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="F231" s="0" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="F232" s="0" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="F233" s="0" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="F234" s="0" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="F235" s="0" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="F236" s="0" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>674</v>
+        <v>726</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>722</v>
+        <v>727</v>
       </c>
       <c r="F237" s="0" t="s">
-        <v>723</v>
+        <v>728</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="F238" s="0" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="F239" s="0" t="s">
-        <v>731</v>
+        <v>736</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>733</v>
+        <v>690</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="F240" s="0" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>690</v>
+        <v>741</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="F241" s="0" t="s">
-        <v>738</v>
+        <v>743</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>694</v>
+        <v>745</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="F242" s="0" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="F243" s="0" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>747</v>
+        <v>706</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>748</v>
+        <v>753</v>
       </c>
       <c r="F244" s="0" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>674</v>
+        <v>710</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="F245" s="0" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
       <c r="F246" s="0" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="F247" s="0" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="B248" s="0" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
       <c r="F248" s="0" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>690</v>
+        <v>770</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>764</v>
+        <v>771</v>
       </c>
       <c r="F249" s="0" t="s">
-        <v>765</v>
+        <v>772</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>694</v>
+        <v>745</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>767</v>
+        <v>774</v>
       </c>
       <c r="F250" s="0" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>769</v>
+        <v>776</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>770</v>
+        <v>702</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
       <c r="F251" s="0" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>774</v>
+        <v>706</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="F252" s="0" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>777</v>
+        <v>782</v>
       </c>
       <c r="B253" s="0" t="s">
-        <v>778</v>
+        <v>710</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="F253" s="0" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="F254" s="0" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="F255" s="0" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="F256" s="0" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="B257" s="0" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="F257" s="0" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="B258" s="0" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="C258" s="0" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="F258" s="0" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="B259" s="0" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="F259" s="0" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="B260" s="0" t="s">
-        <v>782</v>
+        <v>810</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>783</v>
+        <v>811</v>
       </c>
       <c r="F260" s="0" t="s">
-        <v>784</v>
+        <v>812</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>806</v>
+        <v>813</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>786</v>
+        <v>814</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>787</v>
+        <v>815</v>
       </c>
       <c r="F261" s="0" t="s">
-        <v>788</v>
+        <v>816</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>807</v>
+        <v>817</v>
       </c>
       <c r="B262" s="0" t="s">
-        <v>790</v>
+        <v>818</v>
       </c>
       <c r="C262" s="0" t="s">
-        <v>791</v>
+        <v>819</v>
       </c>
       <c r="F262" s="0" t="s">
-        <v>792</v>
+        <v>820</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>808</v>
+        <v>821</v>
       </c>
       <c r="B263" s="0" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="C263" s="0" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="F263" s="0" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>809</v>
+        <v>822</v>
       </c>
       <c r="B264" s="0" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="C264" s="0" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="F264" s="0" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>813</v>
+        <v>823</v>
       </c>
       <c r="B265" s="0" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="C265" s="0" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="F265" s="0" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>817</v>
+        <v>824</v>
       </c>
       <c r="B266" s="0" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="F266" s="0" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="B267" s="0" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
       <c r="C267" s="0" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="F267" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="B268" s="0" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="F268" s="0" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="B269" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C269" s="0" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="F269" s="0" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="B270" s="0" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="C270" s="0" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="F270" s="0" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
       <c r="B271" s="0" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="F271" s="0" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
       <c r="B272" s="0" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="C272" s="0" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="F272" s="0" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
       <c r="B273" s="0" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="C273" s="0" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="F273" s="0" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="B274" s="0" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="C274" s="0" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="F274" s="0" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="B275" s="0" t="s">
-        <v>854</v>
-      </c>
-      <c r="C275" s="6" t="s">
-        <v>855</v>
-      </c>
-      <c r="F275" s="8" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>858</v>
+      </c>
+      <c r="C275" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="F275" s="0" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="B276" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="C276" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="F276" s="0" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>857</v>
+        <v>865</v>
       </c>
       <c r="B277" s="0" t="s">
-        <v>858</v>
-      </c>
-      <c r="C277" s="3" t="s">
-        <v>859</v>
-      </c>
-      <c r="F277" s="3" t="s">
-        <v>860</v>
+        <v>866</v>
+      </c>
+      <c r="C277" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="F277" s="0" t="s">
+        <v>868</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>861</v>
+        <v>869</v>
       </c>
       <c r="B278" s="0" t="s">
-        <v>862</v>
-      </c>
-      <c r="C278" s="3" t="s">
-        <v>863</v>
-      </c>
-      <c r="F278" s="3" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="0" t="s">
-        <v>865</v>
-      </c>
-      <c r="B279" s="0" t="s">
-        <v>866</v>
-      </c>
-      <c r="C279" s="3" t="s">
-        <v>867</v>
-      </c>
-      <c r="F279" s="3" t="s">
-        <v>868</v>
+        <v>870</v>
+      </c>
+      <c r="C278" s="6" t="s">
+        <v>871</v>
+      </c>
+      <c r="F278" s="8" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="F280" s="3" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="B281" s="0" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="F281" s="3" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="B282" s="0" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c r="C282" s="3" t="s">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c r="F282" s="3" t="s">
-        <v>880</v>
+        <v>884</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="B283" s="0" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>883</v>
+        <v>887</v>
       </c>
       <c r="F283" s="3" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
       <c r="B284" s="0" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="F284" s="3" t="s">
-        <v>888</v>
+        <v>892</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="B285" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>891</v>
+        <v>895</v>
       </c>
       <c r="F285" s="3" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="287" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>897</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>898</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="F286" s="3" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>893</v>
+        <v>901</v>
       </c>
       <c r="B287" s="0" t="s">
-        <v>894</v>
+        <v>902</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>895</v>
+        <v>903</v>
       </c>
       <c r="F287" s="3" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>897</v>
+        <v>905</v>
       </c>
       <c r="B288" s="0" t="s">
-        <v>898</v>
+        <v>906</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="F288" s="3" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="0" t="s">
-        <v>901</v>
-      </c>
-      <c r="B289" s="0" t="s">
-        <v>902</v>
-      </c>
-      <c r="C289" s="3" t="s">
-        <v>903</v>
-      </c>
-      <c r="F289" s="3" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>905</v>
+        <v>909</v>
       </c>
       <c r="B290" s="0" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="F290" s="3" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>913</v>
+      </c>
+      <c r="B291" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="F291" s="3" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="B292" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="E292" s="0" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>918</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="F292" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>912</v>
+        <v>921</v>
       </c>
       <c r="B293" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="E293" s="0" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="0" t="s">
-        <v>915</v>
-      </c>
-      <c r="B294" s="0" t="s">
-        <v>916</v>
-      </c>
-      <c r="E294" s="0" t="s">
-        <v>917</v>
+        <v>922</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="F293" s="3" t="s">
+        <v>924</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>918</v>
+        <v>925</v>
       </c>
       <c r="B295" s="0" t="s">
-        <v>919</v>
+        <v>926</v>
       </c>
       <c r="E295" s="0" t="s">
-        <v>920</v>
+        <v>927</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="10" t="s">
-        <v>921</v>
+      <c r="A296" s="0" t="s">
+        <v>928</v>
       </c>
       <c r="B296" s="0" t="s">
-        <v>922</v>
+        <v>929</v>
       </c>
       <c r="E296" s="0" t="s">
-        <v>923</v>
+        <v>930</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>924</v>
+        <v>931</v>
       </c>
       <c r="B297" s="0" t="s">
-        <v>925</v>
+        <v>932</v>
       </c>
       <c r="E297" s="0" t="s">
-        <v>926</v>
+        <v>933</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>927</v>
+        <v>934</v>
       </c>
       <c r="B298" s="0" t="s">
-        <v>928</v>
+        <v>935</v>
       </c>
       <c r="E298" s="0" t="s">
-        <v>929</v>
+        <v>936</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="0" t="s">
-        <v>930</v>
+      <c r="A299" s="9" t="s">
+        <v>937</v>
       </c>
       <c r="B299" s="0" t="s">
-        <v>931</v>
+        <v>938</v>
       </c>
       <c r="E299" s="0" t="s">
-        <v>932</v>
+        <v>939</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>933</v>
+        <v>940</v>
       </c>
       <c r="B300" s="0" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="E300" s="0" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="302" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="6" t="s">
-        <v>936</v>
+        <v>942</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="s">
+        <v>943</v>
+      </c>
+      <c r="B301" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="E301" s="0" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="s">
+        <v>946</v>
       </c>
       <c r="B302" s="0" t="s">
-        <v>937</v>
-      </c>
-      <c r="C302" s="3" t="s">
-        <v>938</v>
-      </c>
-      <c r="D302" s="0" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="E302" s="0" t="s">
-        <v>937</v>
-      </c>
-      <c r="F302" s="3" t="s">
-        <v>940</v>
-      </c>
-      <c r="G302" s="0" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="6" t="s">
-        <v>942</v>
+      <c r="A303" s="0" t="s">
+        <v>949</v>
       </c>
       <c r="B303" s="0" t="s">
-        <v>943</v>
-      </c>
-      <c r="C303" s="0" t="s">
-        <v>944</v>
+        <v>950</v>
       </c>
       <c r="E303" s="0" t="s">
-        <v>943</v>
-      </c>
-      <c r="F303" s="0" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="6" t="s">
-        <v>946</v>
-      </c>
-      <c r="B304" s="0" t="s">
-        <v>947</v>
-      </c>
-      <c r="C304" s="0" t="s">
-        <v>948</v>
-      </c>
-      <c r="E304" s="0" t="s">
-        <v>947</v>
-      </c>
-      <c r="F304" s="0" t="s">
-        <v>949</v>
+        <v>951</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="B305" s="0" t="s">
+        <v>953</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="D305" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="E305" s="0" t="s">
+        <v>953</v>
+      </c>
+      <c r="F305" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="G305" s="0" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="6" t="s">
+        <v>958</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="C306" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="E306" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="F306" s="0" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="6" t="s">
+        <v>962</v>
+      </c>
+      <c r="B307" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="C307" s="0" t="s">
+        <v>964</v>
+      </c>
+      <c r="E307" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="F307" s="0" t="s">
+        <v>965</v>
       </c>
     </row>
   </sheetData>
@@ -8819,27 +8915,27 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>950</v>
+        <v>966</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>951</v>
+        <v>967</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>952</v>
+        <v>968</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>953</v>
+        <v>969</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>954</v>
+        <v>970</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#xxxxx Add more logs settings in CONFIGURATION, for debugging
</commit_message>
<xml_diff>
--- a/RuntimeResources/System/resources.xlsx
+++ b/RuntimeResources/System/resources.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="1067">
   <si>
     <t xml:space="preserve">stringName</t>
   </si>
@@ -1494,6 +1494,130 @@
     <t xml:space="preserve">Traceログ出力：\n
 DTXManiaLog.txt にログを出力します。\n
 この設定の変更は、DTXMania の再起動後に有効となります。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strCfgSysLogEnumerateSongs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnumerateSongsLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For debugging:\n
+Turn ON to put song enumeration logs to DTXManiaLog.txt.\n
+If you have no problems, leave it OFF.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">デバッグ用:\n
+ON にすると、DTXManiaLog.txt に曲データ検索と登録の詳細なログを出力します。\n
+通常はOFFのままお使いください。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strCfgSysLogCreateRelease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CreateReleaseLog</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">For debugging:\n
+Turn ON to put new/dispose logs about audio/texture to DTXManiaLog.txt.\n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">If you have no problems, leave it OFF.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">デバッグ用:\n
+ON にすると、DTXManiaLog.txt にサウンドやテクスチャに関する生成/破棄のログを出力します。\n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">通常はOFFのままお使いください。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">strCfgSysLogDTX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChipLog</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">For debugging:\n
+Turn ON to put DTX chip logs to DTXManiaLog.txt.\n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">If you have no problems, leave it OFF.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">デバッグ用:\n
+ON にすると、DTXManiaLog.txt にDTXデータをチップのリストに変換した結果の詳細なログを出力します。\n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">通常はOFFのままお使いください。</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">strCfgSysSoundDeviceType</t>
@@ -6747,7 +6871,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -6806,9 +6930,23 @@
     </font>
     <font>
       <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="MS Gothic"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
       <color rgb="FFA31515"/>
       <name val="MS Gothic"/>
       <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="MS Gothic"/>
+      <family val="0"/>
       <charset val="128"/>
     </font>
     <font>
@@ -6908,7 +7046,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6945,7 +7083,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6973,7 +7119,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6981,19 +7127,19 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7074,13 +7220,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J327"/>
+  <dimension ref="A1:J330"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A171" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C116" activeCellId="0" sqref="C116"/>
+      <selection pane="topLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.51"/>
@@ -8233,7 +8379,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="128.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>269</v>
       </c>
@@ -8243,60 +8389,60 @@
       <c r="C84" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="F84" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="F84" s="8" t="s">
+    </row>
+    <row r="85" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G84" s="6" t="s">
+      <c r="B85" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="H84" s="6"/>
-    </row>
-    <row r="85" customFormat="false" ht="128.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="C85" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="F85" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C85" s="8" t="s">
+    </row>
+    <row r="86" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="F85" s="8" t="s">
+      <c r="B86" s="0" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="6" t="s">
+      <c r="C86" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="F86" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="C86" s="8" t="s">
+    </row>
+    <row r="87" customFormat="false" ht="128.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="F86" s="8" t="s">
+      <c r="B87" s="0" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="C87" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="D87" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="F87" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="G87" s="6" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="108.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" customFormat="false" ht="128.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>287</v>
       </c>
@@ -8310,8 +8456,8 @@
         <v>290</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="89" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="6" t="s">
         <v>291</v>
       </c>
       <c r="B89" s="0" t="s">
@@ -8324,7 +8470,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>295</v>
       </c>
@@ -8338,11 +8484,11 @@
         <v>298</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="6" t="s">
+    <row r="91" customFormat="false" ht="108.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="0" t="s">
         <v>300</v>
       </c>
       <c r="C91" s="8" t="s">
@@ -8352,11 +8498,11 @@
         <v>302</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="9" t="s">
+    <row r="92" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="0" t="s">
         <v>304</v>
       </c>
       <c r="C92" s="8" t="s">
@@ -8366,11 +8512,11 @@
         <v>306</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="0" t="s">
         <v>308</v>
       </c>
       <c r="C93" s="8" t="s">
@@ -8380,8 +8526,8 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+    <row r="94" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="6" t="s">
         <v>311</v>
       </c>
       <c r="B94" s="6" t="s">
@@ -8394,8 +8540,8 @@
         <v>314</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+    <row r="95" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="11" t="s">
         <v>315</v>
       </c>
       <c r="B95" s="6" t="s">
@@ -8408,82 +8554,82 @@
         <v>318</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="B96" s="6"/>
+      <c r="B96" s="6" t="s">
+        <v>320</v>
+      </c>
       <c r="C96" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="F96" s="8"/>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="6"/>
-      <c r="C97" s="8"/>
-      <c r="F97" s="8"/>
+        <v>321</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="10" t="s">
-        <v>321</v>
+      <c r="A98" s="0" t="s">
+        <v>327</v>
       </c>
       <c r="B98" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B99" s="6"/>
+      <c r="C99" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="F99" s="8"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="6"/>
+      <c r="C100" s="8"/>
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C101" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F98" s="6" t="s">
+      <c r="F101" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="10"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="F99" s="6"/>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="F100" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="F101" s="0" t="s">
-        <v>329</v>
-      </c>
-    </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>333</v>
-      </c>
+      <c r="A102" s="12"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="F102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
@@ -8503,61 +8649,61 @@
       <c r="A104" s="0" t="s">
         <v>338</v>
       </c>
+      <c r="B104" s="6" t="s">
+        <v>339</v>
+      </c>
       <c r="C104" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="C105" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="F105" s="0" t="s">
-        <v>337</v>
+        <v>342</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="C108" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="F108" s="6" t="s">
+      <c r="C108" s="0" t="s">
         <v>353</v>
+      </c>
+      <c r="F108" s="0" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8609,137 +8755,137 @@
       <c r="B112" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="C112" s="0" t="s">
+      <c r="C112" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="F112" s="0" t="s">
+      <c r="F112" s="6" t="s">
         <v>369</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="B114" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>375</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="F115" s="8" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="69.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
         <v>379</v>
       </c>
-      <c r="B116" s="6" t="s">
+      <c r="C115" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="C116" s="8" t="s">
+      <c r="F115" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="F116" s="8" t="s">
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="117" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="B117" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="C117" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="F117" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="F117" s="8" t="s">
+    </row>
+    <row r="118" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="6"/>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="10" t="s">
+      <c r="B118" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="C118" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="69.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="6"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="B123" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C120" s="6" t="s">
+      <c r="C123" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F120" s="6" t="s">
+      <c r="F123" s="6" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="F122" s="0" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="F123" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="F124" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>400</v>
+        <v>335</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>401</v>
@@ -8776,65 +8922,65 @@
         <v>410</v>
       </c>
     </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="F128" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>323</v>
+        <v>416</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>392</v>
+        <v>420</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="F130" s="0" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="B131" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="F131" s="0" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>400</v>
+        <v>335</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>401</v>
+        <v>424</v>
       </c>
       <c r="F132" s="0" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>404</v>
@@ -8843,12 +8989,12 @@
         <v>405</v>
       </c>
       <c r="F133" s="0" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>408</v>
@@ -8857,615 +9003,615 @@
         <v>409</v>
       </c>
       <c r="F134" s="0" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="F135" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="B136" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="F136" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>432</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="F136" s="0" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="F137" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>429</v>
-      </c>
-      <c r="C139" s="0" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="122.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="B140" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="C140" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="D140" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="F140" s="8" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
-        <v>435</v>
-      </c>
-      <c r="B141" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="C141" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="D141" s="6" t="s">
+      <c r="C139" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="F141" s="8" t="s">
+      <c r="F139" s="3" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>440</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>441</v>
       </c>
-      <c r="C142" s="8" t="s">
+      <c r="C142" s="0" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="122.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
         <v>442</v>
       </c>
-      <c r="D142" s="6" t="s">
+      <c r="B143" s="0" t="s">
         <v>443</v>
       </c>
-      <c r="F142" s="8" t="s">
+      <c r="C143" s="8" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="143" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+      <c r="D143" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="B143" s="0" t="s">
+      <c r="F143" s="8" t="s">
         <v>446</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="D143" s="6" t="s">
-        <v>448</v>
-      </c>
-      <c r="F143" s="8" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="D144" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B144" s="0" t="s">
+      <c r="F144" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="C144" s="8" t="s">
+    </row>
+    <row r="145" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="F144" s="8" t="s">
+      <c r="B145" s="0" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="145" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
+      <c r="C145" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="B145" s="0" t="s">
+      <c r="D145" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="C145" s="8" t="s">
+      <c r="F145" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="D145" s="6" t="s">
+    </row>
+    <row r="146" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="F145" s="8" t="s">
+      <c r="B146" s="0" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="146" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="C146" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="B146" s="0" t="s">
+      <c r="D146" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="F146" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="D146" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="F146" s="8" t="s">
+    </row>
+    <row r="147" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="B147" s="0" t="s">
         <v>463</v>
       </c>
-      <c r="B147" s="0" t="s">
+      <c r="C147" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="C147" s="8" t="s">
+      <c r="F147" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="D147" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="F147" s="8" t="s">
+    </row>
+    <row r="148" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="149" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="D148" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="F148" s="8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="C149" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="D149" s="6" t="s">
         <v>469</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="D150" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="F150" s="8" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="F152" s="3" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
-        <v>476</v>
-      </c>
-      <c r="B153" s="0" t="s">
-        <v>477</v>
+        <v>481</v>
+      </c>
+      <c r="F152" s="8" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="B154" s="0" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="C156" s="8" t="s">
-        <v>481</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="F156" s="3" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="C157" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="F157" s="0" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="B158" s="0" t="s">
         <v>489</v>
       </c>
-      <c r="C158" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="F158" s="6" t="s">
+    </row>
+    <row r="159" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="159" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
+      <c r="B159" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="B159" s="0" t="s">
+      <c r="C159" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="C159" s="8" t="s">
+      <c r="D159" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="F159" s="8" t="s">
+      <c r="F159" s="3" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>496</v>
       </c>
-      <c r="B160" s="6" t="s">
+      <c r="B160" s="0" t="s">
         <v>497</v>
       </c>
-      <c r="C160" s="8" t="s">
+      <c r="C160" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="D160" s="6" t="s">
+      <c r="F160" s="0" t="s">
         <v>499</v>
-      </c>
-      <c r="F160" s="8" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B161" s="0" t="s">
         <v>501</v>
       </c>
-      <c r="B161" s="0" t="s">
+      <c r="C161" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="C161" s="6" t="s">
+      <c r="F161" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="F161" s="0" t="s">
+    </row>
+    <row r="162" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
+      <c r="B162" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="B162" s="0" t="s">
+      <c r="C162" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="C162" s="6" t="s">
+      <c r="F162" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="D162" s="6"/>
-      <c r="F162" s="0" t="s">
+    </row>
+    <row r="163" customFormat="false" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
         <v>508</v>
       </c>
-      <c r="J162" s="4" t="s">
+      <c r="B163" s="6" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="163" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="11" t="s">
+      <c r="C163" s="8" t="s">
         <v>510</v>
       </c>
-      <c r="B163" s="11" t="s">
+      <c r="D163" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="C163" s="12" t="s">
+      <c r="F163" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="D163" s="12" t="s">
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
         <v>513</v>
       </c>
-      <c r="F163" s="12" t="s">
+      <c r="B164" s="0" t="s">
         <v>514</v>
       </c>
-      <c r="J163" s="14" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="10" t="s">
+      <c r="C164" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="B164" s="10" t="s">
+      <c r="F164" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="C164" s="6" t="s">
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="D164" s="6" t="s">
+      <c r="B165" s="0" t="s">
         <v>518</v>
       </c>
-      <c r="F164" s="6" t="s">
+      <c r="C165" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="J164" s="4"/>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="10" t="s">
-        <v>516</v>
-      </c>
-      <c r="B165" s="10" t="s">
+      <c r="D165" s="6"/>
+      <c r="F165" s="0" t="s">
         <v>520</v>
       </c>
-      <c r="C165" s="6" t="s">
+      <c r="J165" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="D165" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="F165" s="6" t="s">
+    </row>
+    <row r="166" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="13" t="s">
         <v>522</v>
       </c>
-      <c r="J165" s="4"/>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="10" t="s">
+      <c r="B166" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="B166" s="10" t="s">
+      <c r="C166" s="14" t="s">
         <v>524</v>
       </c>
-      <c r="C166" s="6" t="s">
+      <c r="D166" s="14" t="s">
         <v>525</v>
       </c>
-      <c r="D166" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="F166" s="6" t="s">
+      <c r="F166" s="14" t="s">
         <v>526</v>
       </c>
-      <c r="J166" s="4"/>
+      <c r="J166" s="16" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
+      <c r="A167" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="B167" s="0" t="s">
+      <c r="B167" s="12" t="s">
         <v>528</v>
       </c>
-      <c r="C167" s="0" t="s">
+      <c r="C167" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="F167" s="0" t="s">
+      <c r="D167" s="6" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="168" s="13" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="13" t="s">
+      <c r="F167" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="B168" s="13" t="s">
+      <c r="J167" s="4"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="B168" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="C168" s="15" t="s">
+      <c r="C168" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="D168" s="12" t="s">
+      <c r="D168" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="F168" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="F168" s="15" t="s">
+      <c r="J168" s="4"/>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="12" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="169" s="13" customFormat="true" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="13" t="s">
+      <c r="B169" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="B169" s="13" t="s">
+      <c r="C169" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="C169" s="15" t="s">
+      <c r="D169" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="F169" s="6" t="s">
         <v>538</v>
       </c>
-      <c r="D169" s="12" t="s">
+      <c r="J169" s="4"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
         <v>539</v>
       </c>
-      <c r="F169" s="15" t="s">
+      <c r="B170" s="0" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="170" s="13" customFormat="true" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="13" t="s">
+      <c r="C170" s="0" t="s">
         <v>541</v>
       </c>
-      <c r="B170" s="13" t="s">
+      <c r="F170" s="0" t="s">
         <v>542</v>
       </c>
-      <c r="C170" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="D170" s="12" t="s">
-        <v>539</v>
-      </c>
-      <c r="F170" s="15" t="s">
+    </row>
+    <row r="171" s="15" customFormat="true" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="15" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="172" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
+      <c r="B171" s="15" t="s">
         <v>544</v>
       </c>
-      <c r="B172" s="0" t="s">
+      <c r="C171" s="17" t="s">
         <v>545</v>
       </c>
-      <c r="C172" s="8" t="s">
+      <c r="D171" s="14" t="s">
         <v>546</v>
       </c>
-      <c r="F172" s="3" t="s">
+      <c r="F171" s="17" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
+    <row r="172" s="15" customFormat="true" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="15" t="s">
         <v>548</v>
       </c>
-      <c r="B173" s="0" t="s">
+      <c r="B172" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="C173" s="8" t="s">
+      <c r="C172" s="17" t="s">
         <v>550</v>
       </c>
-      <c r="F173" s="3" t="s">
+      <c r="D172" s="14" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
+      <c r="F172" s="17" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" s="15" customFormat="true" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="B173" s="15" t="s">
+        <v>554</v>
+      </c>
+      <c r="C173" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D173" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="F173" s="17" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>554</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>555</v>
+        <v>557</v>
+      </c>
+      <c r="C175" s="8" t="s">
+        <v>558</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>561</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>559</v>
-      </c>
-      <c r="C178" s="8" t="s">
-        <v>560</v>
-      </c>
-      <c r="F178" s="8" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>565</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="F179" s="3" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="B183" s="16" t="s">
-        <v>566</v>
-      </c>
-      <c r="C183" s="6" t="s">
-        <v>567</v>
-      </c>
-      <c r="F183" s="6" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="B184" s="16" t="s">
+      <c r="B179" s="0" t="s">
         <v>570</v>
       </c>
-      <c r="C184" s="6" t="s">
+    </row>
+    <row r="181" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
         <v>571</v>
       </c>
-      <c r="F184" s="6" t="s">
+      <c r="C181" s="8" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="4" t="s">
+      <c r="F181" s="8" t="s">
         <v>573</v>
       </c>
-      <c r="B185" s="16" t="s">
+    </row>
+    <row r="182" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="186" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
+      <c r="C182" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="B186" s="0" t="s">
+      <c r="F182" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C186" s="3" t="s">
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="F186" s="3" t="s">
+      <c r="B186" s="18" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="187" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
+      <c r="C186" s="6" t="s">
         <v>579</v>
       </c>
-      <c r="B187" s="0" t="s">
+      <c r="F186" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="C187" s="3" t="s">
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="F187" s="3" t="s">
+      <c r="B187" s="18" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="188" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
+      <c r="C187" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="B188" s="0" t="s">
+      <c r="F187" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="C188" s="3" t="s">
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="F188" s="3" t="s">
+      <c r="B188" s="18" t="s">
         <v>586</v>
       </c>
     </row>
@@ -9684,152 +9830,152 @@
         <v>647</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>620</v>
+        <v>648</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>624</v>
+        <v>652</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="F205" s="3" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>628</v>
+        <v>656</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="F206" s="3" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B207" s="0" t="s">
         <v>632</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B208" s="0" t="s">
         <v>636</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="F208" s="3" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B209" s="0" t="s">
         <v>640</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="F209" s="3" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="B210" s="0" t="s">
         <v>644</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>668</v>
-      </c>
-      <c r="B211" s="6" t="s">
-        <v>669</v>
+        <v>671</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>648</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="F212" s="3" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="F213" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>672</v>
-      </c>
-      <c r="B214" s="0" t="s">
-        <v>673</v>
-      </c>
-      <c r="C214" s="6" t="s">
-        <v>674</v>
-      </c>
-      <c r="F214" s="6" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="B215" s="0" t="s">
-        <v>677</v>
-      </c>
-      <c r="C215" s="6" t="s">
-        <v>678</v>
-      </c>
-      <c r="F215" s="6" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
         <v>680</v>
       </c>
-      <c r="B216" s="0" t="s">
+      <c r="B214" s="6" t="s">
         <v>681</v>
       </c>
-      <c r="C216" s="6" t="s">
+      <c r="C214" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="F216" s="6" t="s">
+      <c r="F214" s="3" t="s">
         <v>683</v>
       </c>
     </row>
@@ -9847,86 +9993,86 @@
         <v>687</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
         <v>688</v>
       </c>
       <c r="B218" s="0" t="s">
         <v>689</v>
       </c>
-      <c r="C218" s="8" t="s">
+      <c r="C218" s="6" t="s">
         <v>690</v>
       </c>
       <c r="F218" s="6" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="0" t="s">
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
         <v>692</v>
       </c>
-      <c r="C223" s="0" t="s">
+      <c r="B219" s="0" t="s">
         <v>693</v>
       </c>
-      <c r="F223" s="0" t="s">
+      <c r="C219" s="6" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
+      <c r="F219" s="6" t="s">
         <v>695</v>
       </c>
-      <c r="C224" s="0" t="s">
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
         <v>696</v>
       </c>
-      <c r="F224" s="0" t="s">
+      <c r="B220" s="0" t="s">
         <v>697</v>
       </c>
+      <c r="C220" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="F220" s="6" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>700</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="C221" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="F221" s="6" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="C226" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="F226" s="0" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="17"/>
-    </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="0" t="s">
-        <v>698</v>
-      </c>
-      <c r="B228" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="C228" s="0" t="s">
-        <v>700</v>
-      </c>
-      <c r="F228" s="0" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="0" t="s">
-        <v>702</v>
-      </c>
-      <c r="B229" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="C229" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="F229" s="0" t="s">
-        <v>705</v>
+      <c r="A227" s="0" t="s">
+        <v>707</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>708</v>
+      </c>
+      <c r="F227" s="0" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="B230" s="0" t="s">
-        <v>707</v>
-      </c>
-      <c r="C230" s="0" t="s">
-        <v>708</v>
-      </c>
-      <c r="F230" s="0" t="s">
-        <v>709</v>
-      </c>
+      <c r="C230" s="19"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
@@ -10087,49 +10233,49 @@
         <v>754</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>707</v>
+        <v>755</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="F242" s="0" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="F243" s="0" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="F244" s="0" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>766</v>
+        <v>719</v>
       </c>
       <c r="C245" s="0" t="s">
         <v>767</v>
@@ -10143,213 +10289,213 @@
         <v>769</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F246" s="0" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="F247" s="0" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B248" s="0" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="F248" s="0" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>780</v>
+        <v>735</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F249" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>707</v>
+        <v>739</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="F250" s="0" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F251" s="0" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>762</v>
+        <v>792</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="F252" s="0" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B253" s="0" t="s">
         <v>719</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="F253" s="0" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>723</v>
+        <v>799</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="F254" s="0" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="F255" s="0" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>803</v>
+        <v>731</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="F256" s="0" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B257" s="0" t="s">
-        <v>807</v>
+        <v>735</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="F257" s="0" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="18" t="s">
         <v>810</v>
       </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>811</v>
+      </c>
       <c r="B258" s="0" t="s">
-        <v>811</v>
-      </c>
-      <c r="C258" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="C258" s="0" t="s">
         <v>812</v>
       </c>
-      <c r="F258" s="19" t="s">
+      <c r="F258" s="0" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="9" t="s">
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
         <v>814</v>
       </c>
       <c r="B259" s="0" t="s">
         <v>815</v>
       </c>
-      <c r="C259" s="3" t="s">
+      <c r="C259" s="0" t="s">
         <v>816</v>
       </c>
-      <c r="F259" s="19" t="s">
+      <c r="F259" s="0" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="9" t="s">
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
         <v>818</v>
       </c>
       <c r="B260" s="0" t="s">
         <v>819</v>
       </c>
-      <c r="C260" s="3" t="s">
+      <c r="C260" s="0" t="s">
         <v>820</v>
       </c>
-      <c r="F260" s="19" t="s">
+      <c r="F260" s="0" t="s">
         <v>821</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="9" t="s">
+      <c r="A261" s="20" t="s">
         <v>822</v>
       </c>
       <c r="B261" s="0" t="s">
@@ -10358,12 +10504,12 @@
       <c r="C261" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="F261" s="19" t="s">
+      <c r="F261" s="21" t="s">
         <v>825</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="9" t="s">
+      <c r="A262" s="11" t="s">
         <v>826</v>
       </c>
       <c r="B262" s="0" t="s">
@@ -10372,12 +10518,12 @@
       <c r="C262" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="F262" s="19" t="s">
+      <c r="F262" s="21" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="9" t="s">
+      <c r="A263" s="11" t="s">
         <v>830</v>
       </c>
       <c r="B263" s="0" t="s">
@@ -10386,12 +10532,12 @@
       <c r="C263" s="3" t="s">
         <v>832</v>
       </c>
-      <c r="F263" s="19" t="s">
+      <c r="F263" s="21" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="9" t="s">
+      <c r="A264" s="11" t="s">
         <v>834</v>
       </c>
       <c r="B264" s="0" t="s">
@@ -10400,12 +10546,12 @@
       <c r="C264" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="F264" s="19" t="s">
+      <c r="F264" s="21" t="s">
         <v>837</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="9" t="s">
+      <c r="A265" s="11" t="s">
         <v>838</v>
       </c>
       <c r="B265" s="0" t="s">
@@ -10414,12 +10560,12 @@
       <c r="C265" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="F265" s="19" t="s">
+      <c r="F265" s="21" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="9" t="s">
+      <c r="A266" s="11" t="s">
         <v>842</v>
       </c>
       <c r="B266" s="0" t="s">
@@ -10428,12 +10574,12 @@
       <c r="C266" s="3" t="s">
         <v>844</v>
       </c>
-      <c r="F266" s="19" t="s">
+      <c r="F266" s="21" t="s">
         <v>845</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="9" t="s">
+      <c r="A267" s="11" t="s">
         <v>846</v>
       </c>
       <c r="B267" s="0" t="s">
@@ -10442,12 +10588,12 @@
       <c r="C267" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="F267" s="19" t="s">
+      <c r="F267" s="21" t="s">
         <v>849</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="9" t="s">
+      <c r="A268" s="11" t="s">
         <v>850</v>
       </c>
       <c r="B268" s="0" t="s">
@@ -10456,12 +10602,12 @@
       <c r="C268" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="F268" s="19" t="s">
+      <c r="F268" s="21" t="s">
         <v>853</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="9" t="s">
+      <c r="A269" s="11" t="s">
         <v>854</v>
       </c>
       <c r="B269" s="0" t="s">
@@ -10470,91 +10616,91 @@
       <c r="C269" s="3" t="s">
         <v>856</v>
       </c>
-      <c r="F269" s="19" t="s">
+      <c r="F269" s="21" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="270" s="13" customFormat="true" ht="69.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="20" t="s">
+    <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="11" t="s">
         <v>858</v>
       </c>
-      <c r="B270" s="13" t="s">
+      <c r="B270" s="0" t="s">
         <v>859</v>
       </c>
-      <c r="C270" s="15" t="s">
+      <c r="C270" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="F270" s="15" t="s">
+      <c r="F270" s="21" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="271" s="13" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="20" t="s">
+    <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="11" t="s">
         <v>862</v>
       </c>
-      <c r="B271" s="13" t="s">
+      <c r="B271" s="0" t="s">
         <v>863</v>
       </c>
-      <c r="C271" s="15" t="s">
+      <c r="C271" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="F271" s="15" t="s">
+      <c r="F271" s="21" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="272" s="13" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="20" t="s">
+    <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="11" t="s">
         <v>866</v>
       </c>
-      <c r="B272" s="13" t="s">
+      <c r="B272" s="0" t="s">
         <v>867</v>
       </c>
-      <c r="C272" s="15" t="s">
+      <c r="C272" s="3" t="s">
         <v>868</v>
       </c>
-      <c r="F272" s="15" t="s">
+      <c r="F272" s="21" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="0" t="s">
+    <row r="273" s="15" customFormat="true" ht="69.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="22" t="s">
         <v>870</v>
       </c>
-      <c r="B273" s="0" t="s">
+      <c r="B273" s="15" t="s">
         <v>871</v>
       </c>
-      <c r="C273" s="0" t="s">
+      <c r="C273" s="17" t="s">
         <v>872</v>
       </c>
-      <c r="F273" s="0" t="s">
+      <c r="F273" s="17" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="0" t="s">
+    <row r="274" s="15" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="22" t="s">
         <v>874</v>
       </c>
-      <c r="B274" s="0" t="s">
+      <c r="B274" s="15" t="s">
         <v>875</v>
       </c>
-      <c r="C274" s="0" t="s">
+      <c r="C274" s="17" t="s">
         <v>876</v>
       </c>
-      <c r="F274" s="0" t="s">
+      <c r="F274" s="17" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="0" t="s">
+    <row r="275" s="15" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="22" t="s">
         <v>878</v>
       </c>
-      <c r="B275" s="0" t="s">
+      <c r="B275" s="15" t="s">
         <v>879</v>
       </c>
-      <c r="C275" s="0" t="s">
+      <c r="C275" s="17" t="s">
         <v>880</v>
       </c>
-      <c r="F275" s="0" t="s">
+      <c r="F275" s="17" t="s">
         <v>881</v>
       </c>
     </row>
@@ -10619,46 +10765,46 @@
         <v>898</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>875</v>
+        <v>899</v>
       </c>
       <c r="C280" s="0" t="s">
-        <v>876</v>
+        <v>900</v>
       </c>
       <c r="F280" s="0" t="s">
-        <v>877</v>
+        <v>901</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="B281" s="0" t="s">
-        <v>879</v>
+        <v>903</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>880</v>
+        <v>904</v>
       </c>
       <c r="F281" s="0" t="s">
-        <v>881</v>
+        <v>905</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>900</v>
+        <v>906</v>
       </c>
       <c r="B282" s="0" t="s">
-        <v>883</v>
+        <v>907</v>
       </c>
       <c r="C282" s="0" t="s">
-        <v>884</v>
+        <v>908</v>
       </c>
       <c r="F282" s="0" t="s">
-        <v>885</v>
+        <v>909</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B283" s="0" t="s">
         <v>887</v>
@@ -10672,44 +10818,44 @@
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>902</v>
+        <v>911</v>
       </c>
       <c r="B284" s="0" t="s">
-        <v>903</v>
+        <v>891</v>
       </c>
       <c r="C284" s="0" t="s">
-        <v>904</v>
+        <v>892</v>
       </c>
       <c r="F284" s="0" t="s">
-        <v>905</v>
+        <v>893</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>906</v>
+        <v>912</v>
       </c>
       <c r="B285" s="0" t="s">
-        <v>907</v>
+        <v>895</v>
       </c>
       <c r="C285" s="0" t="s">
-        <v>908</v>
+        <v>896</v>
       </c>
       <c r="F285" s="0" t="s">
-        <v>909</v>
+        <v>897</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="B286" s="0" t="s">
-        <v>911</v>
+        <v>899</v>
       </c>
       <c r="C286" s="0" t="s">
-        <v>912</v>
+        <v>900</v>
       </c>
       <c r="F286" s="0" t="s">
-        <v>913</v>
+        <v>901</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10740,50 +10886,50 @@
         <v>921</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="21" t="s">
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
         <v>922</v>
       </c>
       <c r="B289" s="0" t="s">
         <v>923</v>
       </c>
-      <c r="C289" s="3" t="s">
+      <c r="C289" s="0" t="s">
         <v>924</v>
       </c>
-      <c r="F289" s="3" t="s">
+      <c r="F289" s="0" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="21" t="s">
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
         <v>926</v>
       </c>
       <c r="B290" s="0" t="s">
         <v>927</v>
       </c>
-      <c r="C290" s="3" t="s">
+      <c r="C290" s="0" t="s">
         <v>928</v>
       </c>
-      <c r="F290" s="3" t="s">
+      <c r="F290" s="0" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="21" t="s">
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
         <v>930</v>
       </c>
       <c r="B291" s="0" t="s">
         <v>931</v>
       </c>
-      <c r="C291" s="3" t="s">
+      <c r="C291" s="0" t="s">
         <v>932</v>
       </c>
-      <c r="F291" s="3" t="s">
+      <c r="F291" s="0" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="21" t="s">
+    <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="23" t="s">
         <v>934</v>
       </c>
       <c r="B292" s="0" t="s">
@@ -10795,91 +10941,91 @@
       <c r="F292" s="3" t="s">
         <v>937</v>
       </c>
-      <c r="I292" s="0" t="s">
+    </row>
+    <row r="293" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="23" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="293" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="21" t="s">
+      <c r="B293" s="0" t="s">
         <v>939</v>
       </c>
-      <c r="B293" s="0" t="s">
+      <c r="C293" s="3" t="s">
         <v>940</v>
       </c>
-      <c r="C293" s="3" t="s">
+      <c r="F293" s="3" t="s">
         <v>941</v>
       </c>
-      <c r="F293" s="3" t="s">
+    </row>
+    <row r="294" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="23" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="294" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="21" t="s">
+      <c r="B294" s="0" t="s">
         <v>943</v>
       </c>
-      <c r="B294" s="0" t="s">
+      <c r="C294" s="3" t="s">
         <v>944</v>
       </c>
-      <c r="C294" s="3" t="s">
+      <c r="F294" s="3" t="s">
         <v>945</v>
       </c>
-      <c r="F294" s="3" t="s">
+    </row>
+    <row r="295" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="23" t="s">
         <v>946</v>
       </c>
-    </row>
-    <row r="295" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="0" t="s">
+      <c r="B295" s="0" t="s">
         <v>947</v>
       </c>
-      <c r="B295" s="0" t="s">
+      <c r="C295" s="3" t="s">
         <v>948</v>
       </c>
-      <c r="C295" s="6" t="s">
+      <c r="F295" s="3" t="s">
         <v>949</v>
       </c>
-      <c r="F295" s="8" t="s">
+      <c r="I295" s="0" t="s">
         <v>950</v>
       </c>
     </row>
+    <row r="296" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="23" t="s">
+        <v>951</v>
+      </c>
+      <c r="B296" s="0" t="s">
+        <v>952</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="F296" s="3" t="s">
+        <v>954</v>
+      </c>
+    </row>
     <row r="297" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="0" t="s">
-        <v>951</v>
+      <c r="A297" s="23" t="s">
+        <v>955</v>
       </c>
       <c r="B297" s="0" t="s">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>953</v>
+        <v>957</v>
       </c>
       <c r="F297" s="3" t="s">
-        <v>954</v>
+        <v>958</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="B298" s="0" t="s">
-        <v>956</v>
-      </c>
-      <c r="C298" s="3" t="s">
-        <v>957</v>
-      </c>
-      <c r="F298" s="3" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="299" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="0" t="s">
-        <v>959</v>
-      </c>
-      <c r="B299" s="0" t="s">
         <v>960</v>
       </c>
-      <c r="C299" s="3" t="s">
+      <c r="C298" s="6" t="s">
         <v>961</v>
       </c>
-      <c r="F299" s="3" t="s">
+      <c r="F298" s="8" t="s">
         <v>962</v>
       </c>
     </row>
@@ -10967,45 +11113,45 @@
         <v>986</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
+        <v>987</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>988</v>
+      </c>
+      <c r="C306" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="F306" s="3" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>987</v>
+        <v>991</v>
       </c>
       <c r="B307" s="0" t="s">
-        <v>988</v>
+        <v>992</v>
       </c>
       <c r="C307" s="3" t="s">
-        <v>989</v>
+        <v>993</v>
       </c>
       <c r="F307" s="3" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="308" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="B308" s="0" t="s">
-        <v>992</v>
+        <v>996</v>
       </c>
       <c r="C308" s="3" t="s">
-        <v>993</v>
+        <v>997</v>
       </c>
       <c r="F308" s="3" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="309" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="0" t="s">
-        <v>995</v>
-      </c>
-      <c r="B309" s="0" t="s">
-        <v>996</v>
-      </c>
-      <c r="C309" s="3" t="s">
-        <v>997</v>
-      </c>
-      <c r="F309" s="3" t="s">
         <v>998</v>
       </c>
     </row>
@@ -11023,182 +11169,224 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B311" s="0" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C311" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F311" s="3" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>1003</v>
+        <v>1007</v>
       </c>
       <c r="B312" s="0" t="s">
-        <v>1004</v>
-      </c>
-      <c r="E312" s="0" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1008</v>
+      </c>
+      <c r="C312" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F312" s="3" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="B313" s="0" t="s">
-        <v>1007</v>
-      </c>
-      <c r="E313" s="0" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="0" t="s">
-        <v>1009</v>
-      </c>
-      <c r="B314" s="0" t="s">
-        <v>1010</v>
-      </c>
-      <c r="E314" s="0" t="s">
-        <v>1011</v>
+        <v>1012</v>
+      </c>
+      <c r="C313" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F313" s="3" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
       <c r="B315" s="0" t="s">
-        <v>1013</v>
+        <v>1016</v>
       </c>
       <c r="E315" s="0" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="10" t="s">
-        <v>1015</v>
+      <c r="A316" s="0" t="s">
+        <v>1018</v>
       </c>
       <c r="B316" s="0" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
       <c r="E316" s="0" t="s">
-        <v>1017</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="B317" s="0" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
       <c r="E317" s="0" t="s">
-        <v>1020</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="B318" s="0" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="E318" s="0" t="s">
-        <v>1023</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="0" t="s">
-        <v>1024</v>
+      <c r="A319" s="12" t="s">
+        <v>1027</v>
       </c>
       <c r="B319" s="0" t="s">
-        <v>1025</v>
+        <v>1028</v>
       </c>
       <c r="E319" s="0" t="s">
-        <v>1026</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>1027</v>
+        <v>1030</v>
       </c>
       <c r="B320" s="0" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
       <c r="E320" s="0" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="6" t="s">
-        <v>1030</v>
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B321" s="0" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E321" s="0" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="s">
+        <v>1036</v>
       </c>
       <c r="B322" s="0" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C322" s="3" t="s">
-        <v>1032</v>
-      </c>
-      <c r="D322" s="0" t="s">
-        <v>1033</v>
+        <v>1037</v>
       </c>
       <c r="E322" s="0" t="s">
-        <v>1031</v>
-      </c>
-      <c r="F322" s="3" t="s">
-        <v>1034</v>
-      </c>
-      <c r="G322" s="0" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="6" t="s">
-        <v>1036</v>
+      <c r="A323" s="0" t="s">
+        <v>1039</v>
       </c>
       <c r="B323" s="0" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C323" s="0" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="E323" s="0" t="s">
-        <v>1037</v>
-      </c>
-      <c r="F323" s="0" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="6" t="s">
-        <v>1040</v>
-      </c>
-      <c r="B324" s="0" t="s">
         <v>1041</v>
       </c>
-      <c r="C324" s="0" t="s">
+    </row>
+    <row r="325" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="6" t="s">
         <v>1042</v>
       </c>
-      <c r="E324" s="0" t="s">
-        <v>1041</v>
-      </c>
-      <c r="F324" s="0" t="s">
+      <c r="B325" s="0" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="326" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A326" s="0" t="s">
+      <c r="C325" s="3" t="s">
         <v>1044</v>
       </c>
-      <c r="C326" s="3" t="s">
+      <c r="D325" s="0" t="s">
         <v>1045</v>
       </c>
-      <c r="F326" s="3" t="s">
+      <c r="E325" s="0" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F325" s="3" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="327" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="0" t="s">
+      <c r="G325" s="0" t="s">
         <v>1047</v>
       </c>
-      <c r="C327" s="3" t="s">
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="6" t="s">
         <v>1048</v>
       </c>
-      <c r="F327" s="3" t="s">
+      <c r="B326" s="0" t="s">
         <v>1049</v>
+      </c>
+      <c r="C326" s="0" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E326" s="0" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F326" s="0" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="6" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B327" s="0" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C327" s="0" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E327" s="0" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F327" s="0" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C329" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F329" s="3" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C330" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F330" s="3" t="s">
+        <v>1061</v>
       </c>
     </row>
   </sheetData>
@@ -11223,34 +11411,34 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="82.08"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1050</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1051</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1052</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1053</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1054</v>
+        <v>1066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>